<commit_message>
Develop ensemble model for final results
</commit_message>
<xml_diff>
--- a/Datasets/results_full.xlsx
+++ b/Datasets/results_full.xlsx
@@ -477,10 +477,10 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>40.57152937025953</v>
+        <v>38.82603207464188</v>
       </c>
       <c r="E2" t="n">
-        <v>-1275945.375</v>
+        <v>-1188835.011349667</v>
       </c>
     </row>
     <row r="3">
@@ -500,10 +500,10 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>33.06654642467952</v>
+        <v>33.82565791732615</v>
       </c>
       <c r="E3" t="n">
-        <v>-1014541.125</v>
+        <v>-1014541.525934224</v>
       </c>
     </row>
     <row r="4">
@@ -523,10 +523,10 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>28.89170423621823</v>
+        <v>30.99823694430878</v>
       </c>
       <c r="E4" t="n">
-        <v>-636951.375</v>
+        <v>-614977.330991718</v>
       </c>
     </row>
     <row r="5">
@@ -546,10 +546,10 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>2.494511505031384</v>
+        <v>16.22681908322957</v>
       </c>
       <c r="E5" t="n">
-        <v>-37596.359375</v>
+        <v>-309615.2685212554</v>
       </c>
     </row>
     <row r="6">
@@ -569,10 +569,10 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>2.60139529383943</v>
+        <v>14.13922243651796</v>
       </c>
       <c r="E6" t="n">
-        <v>-14402.552734375</v>
+        <v>-219310.2006919099</v>
       </c>
     </row>
     <row r="7">
@@ -592,10 +592,10 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>36.1356476619929</v>
+        <v>35.87151118214025</v>
       </c>
       <c r="E7" t="n">
-        <v>-948180.4375</v>
+        <v>-947682.1563098977</v>
       </c>
     </row>
     <row r="8">
@@ -615,10 +615,10 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>28.60110706106323</v>
+        <v>30.69634077797294</v>
       </c>
       <c r="E8" t="n">
-        <v>-819794</v>
+        <v>-809515.3688860169</v>
       </c>
     </row>
     <row r="9">
@@ -638,10 +638,10 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>28.89170423621823</v>
+        <v>29.45350707573782</v>
       </c>
       <c r="E9" t="n">
-        <v>-420265.34375</v>
+        <v>-411545.6223935362</v>
       </c>
     </row>
     <row r="10">
@@ -661,10 +661,10 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3.287128914228693</v>
+        <v>16.75092434359108</v>
       </c>
       <c r="E10" t="n">
-        <v>-39170.05859375</v>
+        <v>-256658.0964985974</v>
       </c>
     </row>
     <row r="11">
@@ -684,10 +684,10 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>3.054753129461777</v>
+        <v>14.54501201713191</v>
       </c>
       <c r="E11" t="n">
-        <v>-9827.619140625</v>
+        <v>-188740.3607194683</v>
       </c>
     </row>
     <row r="12">
@@ -707,10 +707,10 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>100.7620660457243</v>
+        <v>78.39259224291204</v>
       </c>
       <c r="E12" t="n">
-        <v>-2415512</v>
+        <v>-1975429.738784333</v>
       </c>
     </row>
     <row r="13">
@@ -730,10 +730,10 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>96.791666666667</v>
+        <v>74.03363892612992</v>
       </c>
       <c r="E13" t="n">
-        <v>-2305232.25</v>
+        <v>-1951102.050533184</v>
       </c>
     </row>
     <row r="14">
@@ -753,10 +753,10 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>51.05458665329401</v>
+        <v>52.77572075516835</v>
       </c>
       <c r="E14" t="n">
-        <v>-655752.4375</v>
+        <v>-646586.4599556178</v>
       </c>
     </row>
     <row r="15">
@@ -776,10 +776,10 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>73.5113122515012</v>
+        <v>50.00949033119835</v>
       </c>
       <c r="E15" t="n">
-        <v>-947478.125</v>
+        <v>-687173.1145867003</v>
       </c>
     </row>
     <row r="16">
@@ -799,10 +799,10 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>1.57534246575342</v>
+        <v>12.83670887836446</v>
       </c>
       <c r="E16" t="n">
-        <v>-10194.7119140625</v>
+        <v>-285754.0364846688</v>
       </c>
     </row>
     <row r="17">
@@ -822,10 +822,10 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>147.4245115452936</v>
+        <v>109.3941818438427</v>
       </c>
       <c r="E17" t="n">
-        <v>-1951000.25</v>
+        <v>-1667045.262704854</v>
       </c>
     </row>
     <row r="18">
@@ -845,10 +845,10 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>123.7639553429033</v>
+        <v>98.69350734799384</v>
       </c>
       <c r="E18" t="n">
-        <v>-1626073.5</v>
+        <v>-1650101.137704854</v>
       </c>
     </row>
     <row r="19">
@@ -868,10 +868,10 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>67.45902991795138</v>
+        <v>71.24359639498253</v>
       </c>
       <c r="E19" t="n">
-        <v>-1060458</v>
+        <v>-1395774.11472019</v>
       </c>
     </row>
     <row r="20">
@@ -891,10 +891,10 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>71.99295011275102</v>
+        <v>46.45385484777381</v>
       </c>
       <c r="E20" t="n">
-        <v>-716145.25</v>
+        <v>-544706.7459205341</v>
       </c>
     </row>
     <row r="21">
@@ -914,10 +914,10 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>6.799999999999968</v>
+        <v>16.2245674276828</v>
       </c>
       <c r="E21" t="n">
-        <v>-33277.453125</v>
+        <v>-219015.1786025419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>